<commit_message>
My final project with changes
</commit_message>
<xml_diff>
--- a/MyDiagram.xlsx
+++ b/MyDiagram.xlsx
@@ -17,19 +17,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
-    <t>bubbleSortFromFirstToLast</t>
+    <t>mergeSort</t>
   </si>
   <si>
-    <t>bubbleSortFromLastToFirst</t>
+    <t>divByTwoSort</t>
   </si>
   <si>
     <t>shakerSort</t>
   </si>
   <si>
-    <t>divByTwoSort</t>
+    <t>bubbleSortFromFirstToLast</t>
   </si>
   <si>
-    <t>mergeSort</t>
+    <t>bubbleSortFromLastToFirst</t>
   </si>
 </sst>
 </file>
@@ -82,7 +82,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>bubbleSortFromFirstToLast</c:v>
+            <c:v>mergeSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -90,19 +90,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -113,19 +113,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>26986.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30306.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30487.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34570.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35200.0</c:v>
+                  <c:v>42302.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56404.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66472.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91408.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92312.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -135,7 +135,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>bubbleSortFromLastToFirst</c:v>
+            <c:v>divByTwoSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -143,19 +143,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -166,19 +166,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43760.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50892.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>57283.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76298.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100583.0</c:v>
+                  <c:v>22974.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27070.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31389.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42395.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44940.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -196,19 +196,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -219,19 +219,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16410.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19224.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23923.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32117.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33900.0</c:v>
+                  <c:v>13128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20696.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23506.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28117.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41804.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -241,7 +241,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>divByTwoSort</c:v>
+            <c:v>bubbleSortFromFirstToLast</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -249,19 +249,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -272,19 +272,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22610.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24994.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>28290.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28714.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29462.0</c:v>
+                  <c:v>13493.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15849.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21452.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38151.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40311.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,7 +294,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>mergeSort</c:v>
+            <c:v>bubbleSortFromLastToFirst</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -302,19 +302,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -325,19 +325,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53607.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>59365.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72978.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80126.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80306.0</c:v>
+                  <c:v>13858.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21087.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26491.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30082.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31081.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,7 +438,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>bubbleSortFromFirstToLast</c:v>
+            <c:v>mergeSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -446,19 +446,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,19 +469,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22610.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27292.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30046.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32485.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>38711.0</c:v>
+                  <c:v>7659.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7682.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9484.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12881.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19552.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,7 +491,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>bubbleSortFromLastToFirst</c:v>
+            <c:v>divByTwoSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -499,19 +499,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,19 +522,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9846.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10487.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10527.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10992.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11669.0</c:v>
+                  <c:v>7293.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7526.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8411.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16175.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18478.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -552,19 +552,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,19 +575,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12398.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15735.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18075.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24272.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24631.0</c:v>
+                  <c:v>5105.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5947.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6009.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6301.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7113.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,7 +597,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>divByTwoSort</c:v>
+            <c:v>bubbleSortFromFirstToLast</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -605,19 +605,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -628,19 +628,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9846.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10016.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13141.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13607.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15366.0</c:v>
+                  <c:v>5835.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6085.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6475.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10934.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11491.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,7 +650,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>mergeSort</c:v>
+            <c:v>bubbleSortFromLastToFirst</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -658,19 +658,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,19 +681,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19692.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20066.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25018.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25097.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25762.0</c:v>
+                  <c:v>5835.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8423.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13366.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15934.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18394.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -794,7 +794,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>bubbleSortFromFirstToLast</c:v>
+            <c:v>mergeSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -802,19 +802,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,19 +825,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8752.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9117.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11304.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11304.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16530.0</c:v>
+                  <c:v>7293.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7867.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7982.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12108.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17869.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,7 +847,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>bubbleSortFromLastToFirst</c:v>
+            <c:v>divByTwoSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -855,19 +855,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,19 +878,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12399.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15097.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18694.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27086.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27786.0</c:v>
+                  <c:v>6929.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7971.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9870.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10549.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12425.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -908,19 +908,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -931,19 +931,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6564.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6746.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7249.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9075.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11454.0</c:v>
+                  <c:v>5106.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9685.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13879.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17835.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19145.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,7 +953,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>divByTwoSort</c:v>
+            <c:v>bubbleSortFromFirstToLast</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -961,19 +961,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,19 +984,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14222.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14752.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18011.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22341.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25408.0</c:v>
+                  <c:v>7658.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10813.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11367.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14949.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24775.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,7 +1006,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>mergeSort</c:v>
+            <c:v>bubbleSortFromLastToFirst</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -1014,19 +1014,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,19 +1037,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>52877.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>63594.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66687.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80189.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>83643.0</c:v>
+                  <c:v>6199.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8886.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14309.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15857.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18372.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1150,7 +1150,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>bubbleSortFromFirstToLast</c:v>
+            <c:v>mergeSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -1158,19 +1158,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1181,19 +1181,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2205537.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2831321.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3748500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4047524.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4963591.0</c:v>
+                  <c:v>1480204.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2080153.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2188556.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3040531.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4228683.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,7 +1203,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>bubbleSortFromLastToFirst</c:v>
+            <c:v>divByTwoSort</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -1211,19 +1211,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1234,19 +1234,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>374154.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>448019.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>454545.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>455501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>481521.0</c:v>
+                  <c:v>474074.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>477401.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606867.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>979546.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1221435.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,19 +1264,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,19 +1287,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>302313.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>346677.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>432780.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>463686.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>523423.0</c:v>
+                  <c:v>197652.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>267214.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>271374.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>304926.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>305277.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,7 +1309,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>divByTwoSort</c:v>
+            <c:v>bubbleSortFromFirstToLast</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -1317,19 +1317,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,19 +1340,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>515646.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>550319.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>617529.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>665587.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>754048.0</c:v>
+                  <c:v>239225.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245242.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>352375.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>405669.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>566667.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,7 +1362,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>mergeSort</c:v>
+            <c:v>bubbleSortFromLastToFirst</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
@@ -1370,19 +1370,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1393,19 +1393,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>294655.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>338160.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>356739.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>431278.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>477322.0</c:v>
+                  <c:v>195464.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>345607.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>416052.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>519313.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1646,19 +1646,19 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="C1" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="D1" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="E1" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="F1" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="2">
@@ -1666,19 +1666,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>26986.0</v>
+        <v>42302.0</v>
       </c>
       <c r="C2" t="n">
-        <v>30306.0</v>
+        <v>56404.0</v>
       </c>
       <c r="D2" t="n">
-        <v>30487.0</v>
+        <v>66472.0</v>
       </c>
       <c r="E2" t="n">
-        <v>34570.0</v>
+        <v>91408.0</v>
       </c>
       <c r="F2" t="n">
-        <v>35200.0</v>
+        <v>92312.0</v>
       </c>
     </row>
     <row r="3">
@@ -1686,19 +1686,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>43760.0</v>
+        <v>22974.0</v>
       </c>
       <c r="C3" t="n">
-        <v>50892.0</v>
+        <v>27070.0</v>
       </c>
       <c r="D3" t="n">
-        <v>57283.0</v>
+        <v>31389.0</v>
       </c>
       <c r="E3" t="n">
-        <v>76298.0</v>
+        <v>42395.0</v>
       </c>
       <c r="F3" t="n">
-        <v>100583.0</v>
+        <v>44940.0</v>
       </c>
     </row>
     <row r="4">
@@ -1706,19 +1706,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>16410.0</v>
+        <v>13128.0</v>
       </c>
       <c r="C4" t="n">
-        <v>19224.0</v>
+        <v>20696.0</v>
       </c>
       <c r="D4" t="n">
-        <v>23923.0</v>
+        <v>23506.0</v>
       </c>
       <c r="E4" t="n">
-        <v>32117.0</v>
+        <v>28117.0</v>
       </c>
       <c r="F4" t="n">
-        <v>33900.0</v>
+        <v>41804.0</v>
       </c>
     </row>
     <row r="5">
@@ -1726,19 +1726,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>22610.0</v>
+        <v>13493.0</v>
       </c>
       <c r="C5" t="n">
-        <v>24994.0</v>
+        <v>15849.0</v>
       </c>
       <c r="D5" t="n">
-        <v>28290.0</v>
+        <v>21452.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28714.0</v>
+        <v>38151.0</v>
       </c>
       <c r="F5" t="n">
-        <v>29462.0</v>
+        <v>40311.0</v>
       </c>
     </row>
     <row r="6">
@@ -1746,19 +1746,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>53607.0</v>
+        <v>13858.0</v>
       </c>
       <c r="C6" t="n">
-        <v>59365.0</v>
+        <v>21087.0</v>
       </c>
       <c r="D6" t="n">
-        <v>72978.0</v>
+        <v>26491.0</v>
       </c>
       <c r="E6" t="n">
-        <v>80126.0</v>
+        <v>30082.0</v>
       </c>
       <c r="F6" t="n">
-        <v>80306.0</v>
+        <v>31081.0</v>
       </c>
     </row>
   </sheetData>
@@ -1777,19 +1777,19 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="C1" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="D1" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="E1" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="F1" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="2">
@@ -1797,19 +1797,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>22610.0</v>
+        <v>7659.0</v>
       </c>
       <c r="C2" t="n">
-        <v>27292.0</v>
+        <v>7682.0</v>
       </c>
       <c r="D2" t="n">
-        <v>30046.0</v>
+        <v>9484.0</v>
       </c>
       <c r="E2" t="n">
-        <v>32485.0</v>
+        <v>12881.0</v>
       </c>
       <c r="F2" t="n">
-        <v>38711.0</v>
+        <v>19552.0</v>
       </c>
     </row>
     <row r="3">
@@ -1817,19 +1817,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9846.0</v>
+        <v>7293.0</v>
       </c>
       <c r="C3" t="n">
-        <v>10487.0</v>
+        <v>7526.0</v>
       </c>
       <c r="D3" t="n">
-        <v>10527.0</v>
+        <v>8411.0</v>
       </c>
       <c r="E3" t="n">
-        <v>10992.0</v>
+        <v>16175.0</v>
       </c>
       <c r="F3" t="n">
-        <v>11669.0</v>
+        <v>18478.0</v>
       </c>
     </row>
     <row r="4">
@@ -1837,19 +1837,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>12398.0</v>
+        <v>5105.0</v>
       </c>
       <c r="C4" t="n">
-        <v>15735.0</v>
+        <v>5947.0</v>
       </c>
       <c r="D4" t="n">
-        <v>18075.0</v>
+        <v>6009.0</v>
       </c>
       <c r="E4" t="n">
-        <v>24272.0</v>
+        <v>6301.0</v>
       </c>
       <c r="F4" t="n">
-        <v>24631.0</v>
+        <v>7113.0</v>
       </c>
     </row>
     <row r="5">
@@ -1857,19 +1857,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9846.0</v>
+        <v>5835.0</v>
       </c>
       <c r="C5" t="n">
-        <v>10016.0</v>
+        <v>6085.0</v>
       </c>
       <c r="D5" t="n">
-        <v>13141.0</v>
+        <v>6475.0</v>
       </c>
       <c r="E5" t="n">
-        <v>13607.0</v>
+        <v>10934.0</v>
       </c>
       <c r="F5" t="n">
-        <v>15366.0</v>
+        <v>11491.0</v>
       </c>
     </row>
     <row r="6">
@@ -1877,19 +1877,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>19692.0</v>
+        <v>5835.0</v>
       </c>
       <c r="C6" t="n">
-        <v>20066.0</v>
+        <v>8423.0</v>
       </c>
       <c r="D6" t="n">
-        <v>25018.0</v>
+        <v>13366.0</v>
       </c>
       <c r="E6" t="n">
-        <v>25097.0</v>
+        <v>15934.0</v>
       </c>
       <c r="F6" t="n">
-        <v>25762.0</v>
+        <v>18394.0</v>
       </c>
     </row>
   </sheetData>
@@ -1908,19 +1908,19 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="C1" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="D1" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="E1" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="F1" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="2">
@@ -1928,19 +1928,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>8752.0</v>
+        <v>7293.0</v>
       </c>
       <c r="C2" t="n">
-        <v>9117.0</v>
+        <v>7867.0</v>
       </c>
       <c r="D2" t="n">
-        <v>11304.0</v>
+        <v>7982.0</v>
       </c>
       <c r="E2" t="n">
-        <v>11304.0</v>
+        <v>12108.0</v>
       </c>
       <c r="F2" t="n">
-        <v>16530.0</v>
+        <v>17869.0</v>
       </c>
     </row>
     <row r="3">
@@ -1948,19 +1948,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>12399.0</v>
+        <v>6929.0</v>
       </c>
       <c r="C3" t="n">
-        <v>15097.0</v>
+        <v>7971.0</v>
       </c>
       <c r="D3" t="n">
-        <v>18694.0</v>
+        <v>9870.0</v>
       </c>
       <c r="E3" t="n">
-        <v>27086.0</v>
+        <v>10549.0</v>
       </c>
       <c r="F3" t="n">
-        <v>27786.0</v>
+        <v>12425.0</v>
       </c>
     </row>
     <row r="4">
@@ -1968,19 +1968,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>6564.0</v>
+        <v>5106.0</v>
       </c>
       <c r="C4" t="n">
-        <v>6746.0</v>
+        <v>9685.0</v>
       </c>
       <c r="D4" t="n">
-        <v>7249.0</v>
+        <v>13879.0</v>
       </c>
       <c r="E4" t="n">
-        <v>9075.0</v>
+        <v>17835.0</v>
       </c>
       <c r="F4" t="n">
-        <v>11454.0</v>
+        <v>19145.0</v>
       </c>
     </row>
     <row r="5">
@@ -1988,19 +1988,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>14222.0</v>
+        <v>7658.0</v>
       </c>
       <c r="C5" t="n">
-        <v>14752.0</v>
+        <v>10813.0</v>
       </c>
       <c r="D5" t="n">
-        <v>18011.0</v>
+        <v>11367.0</v>
       </c>
       <c r="E5" t="n">
-        <v>22341.0</v>
+        <v>14949.0</v>
       </c>
       <c r="F5" t="n">
-        <v>25408.0</v>
+        <v>24775.0</v>
       </c>
     </row>
     <row r="6">
@@ -2008,19 +2008,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>52877.0</v>
+        <v>6199.0</v>
       </c>
       <c r="C6" t="n">
-        <v>63594.0</v>
+        <v>8886.0</v>
       </c>
       <c r="D6" t="n">
-        <v>66687.0</v>
+        <v>14309.0</v>
       </c>
       <c r="E6" t="n">
-        <v>80189.0</v>
+        <v>15857.0</v>
       </c>
       <c r="F6" t="n">
-        <v>83643.0</v>
+        <v>18372.0</v>
       </c>
     </row>
   </sheetData>
@@ -2039,19 +2039,19 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="C1" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="D1" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="E1" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="F1" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="2">
@@ -2059,19 +2059,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2205537.0</v>
+        <v>1480204.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2831321.0</v>
+        <v>2080153.0</v>
       </c>
       <c r="D2" t="n">
-        <v>3748500.0</v>
+        <v>2188556.0</v>
       </c>
       <c r="E2" t="n">
-        <v>4047524.0</v>
+        <v>3040531.0</v>
       </c>
       <c r="F2" t="n">
-        <v>4963591.0</v>
+        <v>4228683.0</v>
       </c>
     </row>
     <row r="3">
@@ -2079,19 +2079,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>374154.0</v>
+        <v>474074.0</v>
       </c>
       <c r="C3" t="n">
-        <v>448019.0</v>
+        <v>477401.0</v>
       </c>
       <c r="D3" t="n">
-        <v>454545.0</v>
+        <v>606867.0</v>
       </c>
       <c r="E3" t="n">
-        <v>455501.0</v>
+        <v>979546.0</v>
       </c>
       <c r="F3" t="n">
-        <v>481521.0</v>
+        <v>1221435.0</v>
       </c>
     </row>
     <row r="4">
@@ -2099,19 +2099,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>302313.0</v>
+        <v>197652.0</v>
       </c>
       <c r="C4" t="n">
-        <v>346677.0</v>
+        <v>267214.0</v>
       </c>
       <c r="D4" t="n">
-        <v>432780.0</v>
+        <v>271374.0</v>
       </c>
       <c r="E4" t="n">
-        <v>463686.0</v>
+        <v>304926.0</v>
       </c>
       <c r="F4" t="n">
-        <v>523423.0</v>
+        <v>305277.0</v>
       </c>
     </row>
     <row r="5">
@@ -2119,19 +2119,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>515646.0</v>
+        <v>239225.0</v>
       </c>
       <c r="C5" t="n">
-        <v>550319.0</v>
+        <v>245242.0</v>
       </c>
       <c r="D5" t="n">
-        <v>617529.0</v>
+        <v>352375.0</v>
       </c>
       <c r="E5" t="n">
-        <v>665587.0</v>
+        <v>405669.0</v>
       </c>
       <c r="F5" t="n">
-        <v>754048.0</v>
+        <v>566667.0</v>
       </c>
     </row>
     <row r="6">
@@ -2139,19 +2139,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>294655.0</v>
+        <v>195464.0</v>
       </c>
       <c r="C6" t="n">
-        <v>338160.0</v>
+        <v>345607.0</v>
       </c>
       <c r="D6" t="n">
-        <v>356739.0</v>
+        <v>350750.0</v>
       </c>
       <c r="E6" t="n">
-        <v>431278.0</v>
+        <v>416052.0</v>
       </c>
       <c r="F6" t="n">
-        <v>477322.0</v>
+        <v>519313.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>